<commit_message>
Insert draw image into body html outlook
</commit_message>
<xml_diff>
--- a/sisrh/Empregados.xlsx
+++ b/sisrh/Empregados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\analisar t\workspace\send_leyman_email_coletivo\sisrh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8049FA-FBAD-4A4B-AE8F-1A87CA4B60EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2337857-0A9B-4CCB-872E-733E561E7F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
@@ -34,32 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
-  <si>
-    <t>ALAIR LEONARDO JORGE</t>
-  </si>
-  <si>
-    <t>GERSON MEIRA PORTELLA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>GUILHERME MARTINS DOS SANTOS JUNIOR</t>
   </si>
   <si>
-    <t>JACINTO DE SOUZA RIBEIRO</t>
-  </si>
-  <si>
     <t>JOAREZ DE MOURA</t>
   </si>
   <si>
-    <t>LAERCIO PEREIRA DA SILVA</t>
-  </si>
-  <si>
     <t>NIVALDO GALVAO DE OLIVEIRA</t>
   </si>
   <si>
-    <t>SILVANNI FERREIRA LEITE</t>
-  </si>
-  <si>
     <t>Assinatura</t>
   </si>
   <si>
@@ -96,21 +81,6 @@
     <t>c150715;</t>
   </si>
   <si>
-    <t>c150716;</t>
-  </si>
-  <si>
-    <t>c150717;</t>
-  </si>
-  <si>
-    <t>c150718;</t>
-  </si>
-  <si>
-    <t>c150719;</t>
-  </si>
-  <si>
-    <t>c150720;</t>
-  </si>
-  <si>
     <t>AG SÃO SEBASTIAO</t>
   </si>
   <si>
@@ -120,18 +90,6 @@
     <t>AG GAMA</t>
   </si>
   <si>
-    <t>AG SUDOESTE</t>
-  </si>
-  <si>
-    <t>AG ASA NORTE</t>
-  </si>
-  <si>
-    <t>AG BRAZLANDIa</t>
-  </si>
-  <si>
-    <t>AG AGUAS LINDAS</t>
-  </si>
-  <si>
     <t>29/10</t>
   </si>
   <si>
@@ -141,22 +99,7 @@
     <t>29/12</t>
   </si>
   <si>
-    <t>29/13</t>
-  </si>
-  <si>
-    <t>29/14</t>
-  </si>
-  <si>
-    <t>29/15</t>
-  </si>
-  <si>
-    <t>29/16</t>
-  </si>
-  <si>
-    <t>29/17</t>
-  </si>
-  <si>
-    <t>Nome Unidade</t>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -261,16 +204,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83F0A8E5-34CD-49F9-AA87-46E2500285A1}" name="Tabela1" displayName="Tabela1" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{122B5EF1-96BF-4C6E-81B2-C1836FFA134B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
-    <sortCondition ref="B1:B9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83F0A8E5-34CD-49F9-AA87-46E2500285A1}" name="Tabela1" displayName="Tabela1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{122B5EF1-96BF-4C6E-81B2-C1836FFA134B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
+    <sortCondition ref="B1:B4"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{CC6188F6-3698-4DE2-852A-E5B478964637}" name="Nome"/>
     <tableColumn id="15" xr3:uid="{67A00C6D-CD56-48E5-8468-E11E0DF96AF9}" name="Data" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{A915A9F6-B877-426B-8630-3528446C3A4D}" name="Unidade"/>
-    <tableColumn id="4" xr3:uid="{9B133098-0E0A-498A-9E7B-8E3157006963}" name="Nome Unidade"/>
+    <tableColumn id="8" xr3:uid="{A915A9F6-B877-426B-8630-3528446C3A4D}" name="Codigo"/>
+    <tableColumn id="4" xr3:uid="{9B133098-0E0A-498A-9E7B-8E3157006963}" name="Unidade"/>
     <tableColumn id="2" xr3:uid="{655701F0-7A3B-4D44-9BCA-99CF73393122}" name="Matrícula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -574,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98547958-D657-46E7-B850-726EE50AB189}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,155 +535,70 @@
   <sheetData>
     <row r="1" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>4462</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>688</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>4221</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6">
-        <v>643</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7">
-        <v>2893</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8">
-        <v>3052</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -768,27 +626,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -797,24 +655,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AABFCBE3A081344CBD19FDD7D36B97EC" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="65b3017dae72f3457fbfe08cdcab5d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fa4d580a-d01a-42c3-9b98-e13a85c10f62" xmlns:ns4="874b114b-9a7e-49de-8627-5ddbce6c662f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e26fdd407132aebd9a4b758b3c93b41b" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1040,25 +880,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA40C47-9E4B-43D8-AED4-0A7727DB5564}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1076,4 +916,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Divide list to send ocult e-mails
</commit_message>
<xml_diff>
--- a/sisrh/Empregados.xlsx
+++ b/sisrh/Empregados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\analisar t\workspace\send_leyman_email_coletivo\sisrh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2337857-0A9B-4CCB-872E-733E561E7F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADEA329-B8C4-4C60-A07F-8141515E18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>GUILHERME MARTINS DOS SANTOS JUNIOR</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t>Codigo</t>
+  </si>
+  <si>
+    <t>c150716;</t>
+  </si>
+  <si>
+    <t>c150717;</t>
+  </si>
+  <si>
+    <t>c150718;</t>
+  </si>
+  <si>
+    <t>c150719;</t>
+  </si>
+  <si>
+    <t>c150720;</t>
+  </si>
+  <si>
+    <t>c150721;</t>
   </si>
 </sst>
 </file>
@@ -204,8 +222,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83F0A8E5-34CD-49F9-AA87-46E2500285A1}" name="Tabela1" displayName="Tabela1" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{122B5EF1-96BF-4C6E-81B2-C1836FFA134B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83F0A8E5-34CD-49F9-AA87-46E2500285A1}" name="Tabela1" displayName="Tabela1" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{122B5EF1-96BF-4C6E-81B2-C1836FFA134B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
     <sortCondition ref="B1:B4"/>
   </sortState>
@@ -517,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98547958-D657-46E7-B850-726EE50AB189}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +617,108 @@
       </c>
       <c r="E4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>4462</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>688</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>4462</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>688</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -655,6 +775,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AABFCBE3A081344CBD19FDD7D36B97EC" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="65b3017dae72f3457fbfe08cdcab5d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fa4d580a-d01a-42c3-9b98-e13a85c10f62" xmlns:ns4="874b114b-9a7e-49de-8627-5ddbce6c662f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e26fdd407132aebd9a4b758b3c93b41b" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -880,25 +1018,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA40C47-9E4B-43D8-AED4-0A7727DB5564}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -916,22 +1054,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust layout infos in body e-mail
</commit_message>
<xml_diff>
--- a/sisrh/Empregados.xlsx
+++ b/sisrh/Empregados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\analisar t\workspace\send_leyman_email_coletivo\sisrh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADEA329-B8C4-4C60-A07F-8141515E18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBB10F5-77DE-4457-AC74-970EE352AD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{652DF72A-66DF-46A1-927A-2A14980F385E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>GUILHERME MARTINS DOS SANTOS JUNIOR</t>
   </si>
@@ -90,15 +90,6 @@
     <t>AG GAMA</t>
   </si>
   <si>
-    <t>29/10</t>
-  </si>
-  <si>
-    <t>29/11</t>
-  </si>
-  <si>
-    <t>29/12</t>
-  </si>
-  <si>
     <t>Codigo</t>
   </si>
   <si>
@@ -108,16 +99,22 @@
     <t>c150717;</t>
   </si>
   <si>
-    <t>c150718;</t>
-  </si>
-  <si>
-    <t>c150719;</t>
-  </si>
-  <si>
-    <t>c150720;</t>
-  </si>
-  <si>
-    <t>c150721;</t>
+    <t>24/10</t>
+  </si>
+  <si>
+    <t>25/10</t>
+  </si>
+  <si>
+    <t>26/10</t>
+  </si>
+  <si>
+    <t>ARTHUR DE CASTRO</t>
+  </si>
+  <si>
+    <t>WILTON VASQUEZ</t>
+  </si>
+  <si>
+    <t>AILTON MARCELO</t>
   </si>
 </sst>
 </file>
@@ -222,17 +219,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83F0A8E5-34CD-49F9-AA87-46E2500285A1}" name="Tabela1" displayName="Tabela1" ref="A1:E10" totalsRowShown="0">
-  <autoFilter ref="A1:E10" xr:uid="{122B5EF1-96BF-4C6E-81B2-C1836FFA134B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
-    <sortCondition ref="B1:B4"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79A49B1C-F2C7-461D-8F5C-092865E3F43E}" name="Tabela13" displayName="Tabela13" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{79A49B1C-F2C7-461D-8F5C-092865E3F43E}"/>
   <tableColumns count="5">
-    <tableColumn id="3" xr3:uid="{CC6188F6-3698-4DE2-852A-E5B478964637}" name="Nome"/>
-    <tableColumn id="15" xr3:uid="{67A00C6D-CD56-48E5-8468-E11E0DF96AF9}" name="Data" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{A915A9F6-B877-426B-8630-3528446C3A4D}" name="Codigo"/>
-    <tableColumn id="4" xr3:uid="{9B133098-0E0A-498A-9E7B-8E3157006963}" name="Unidade"/>
-    <tableColumn id="2" xr3:uid="{655701F0-7A3B-4D44-9BCA-99CF73393122}" name="Matrícula"/>
+    <tableColumn id="3" xr3:uid="{6BA36F94-53D1-43FE-AD1D-5F0BC42BA99A}" name="Nome"/>
+    <tableColumn id="15" xr3:uid="{EE95C134-555E-46C3-8C76-20C3257D45D0}" name="Data" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{7F491C8C-4EFF-4D82-9712-5EF2CEE25079}" name="Codigo"/>
+    <tableColumn id="4" xr3:uid="{4943D4CF-CECB-4406-AC45-6A08C60F98AA}" name="Unidade"/>
+    <tableColumn id="2" xr3:uid="{DAF11CD6-C8FB-4579-B0F2-3EBB98B60973}" name="Matrícula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -535,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98547958-D657-46E7-B850-726EE50AB189}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +545,7 @@
     <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -559,7 +553,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -568,12 +562,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>4462</v>
@@ -585,12 +579,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -602,12 +596,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>688</v>
@@ -621,10 +615,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>4462</v>
@@ -633,15 +627,15 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -650,75 +644,24 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
-      </c>
-      <c r="C7">
-        <v>688</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>4462</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>688</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -775,24 +718,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AABFCBE3A081344CBD19FDD7D36B97EC" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="65b3017dae72f3457fbfe08cdcab5d5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fa4d580a-d01a-42c3-9b98-e13a85c10f62" xmlns:ns4="874b114b-9a7e-49de-8627-5ddbce6c662f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e26fdd407132aebd9a4b758b3c93b41b" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1018,25 +943,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA40C47-9E4B-43D8-AED4-0A7727DB5564}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1054,4 +979,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF7D4AB7-832D-4E2C-B10A-11961EB6AB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF6B064-3CDA-4685-9D85-ED77979C9B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>